<commit_message>
Added all the data but need to make it  capable  of reading multiple spreadsheets
</commit_message>
<xml_diff>
--- a/SummerWork/All_Reports/Adrian_SD_61_2017-2018_Outdoor_School_Report.xlsx
+++ b/SummerWork/All_Reports/Adrian_SD_61_2017-2018_Outdoor_School_Report.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kotharan\Documents\GitHub\qualtrics_data_py\SummerWork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\qualtrics_data_py\SummerWork\All_Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Adrian School District #61'!$A$1:$H$101</definedName>
     <definedName name="Provider">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="133">
   <si>
     <t>2017-2018 Outdoor School - Reporting Form</t>
   </si>
@@ -457,11 +457,14 @@
   <si>
     <t>In the past, the teacher representing the class that is attending has budjeted for part of Outdoor School with the rest of the funding coming through fundraisers and individual donations.</t>
   </si>
+  <si>
+    <t>abc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -804,6 +807,96 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -813,9 +906,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -827,93 +917,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1208,8 +1211,8 @@
   </sheetPr>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="63" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91:H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1226,15 +1229,15 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -1251,28 +1254,28 @@
       <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
@@ -1288,15 +1291,15 @@
       <c r="A6" s="14">
         <v>1</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
@@ -1312,69 +1315,69 @@
       <c r="A8" s="16">
         <v>2</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="51"/>
+      <c r="D9" s="80"/>
       <c r="E9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="52"/>
-      <c r="H9" s="51"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="80"/>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="51"/>
+      <c r="D10" s="80"/>
       <c r="E10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="52"/>
-      <c r="H10" s="51"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="80"/>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="51"/>
+      <c r="D11" s="80"/>
       <c r="E11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="52"/>
-      <c r="H11" s="51"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="80"/>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
@@ -1404,66 +1407,66 @@
       <c r="A14" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
     </row>
     <row r="17" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
     </row>
     <row r="18" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="57"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="68"/>
       <c r="G18" s="22">
         <v>5</v>
       </c>
@@ -1474,13 +1477,13 @@
     </row>
     <row r="19" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="59"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="70"/>
       <c r="G19" s="22">
         <v>3</v>
       </c>
@@ -1491,13 +1494,13 @@
     </row>
     <row r="20" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="59"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="70"/>
       <c r="G20" s="22">
         <v>4</v>
       </c>
@@ -1508,13 +1511,13 @@
     </row>
     <row r="21" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="59"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="70"/>
       <c r="G21" s="22">
         <v>5</v>
       </c>
@@ -1525,13 +1528,13 @@
     </row>
     <row r="22" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="59"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="70"/>
       <c r="G22" s="22">
         <v>5</v>
       </c>
@@ -1572,15 +1575,15 @@
     </row>
     <row r="25" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
@@ -1758,30 +1761,30 @@
       <c r="A35" s="21">
         <v>5</v>
       </c>
-      <c r="B35" s="61" t="s">
+      <c r="B35" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
       <c r="I35" s="23"/>
       <c r="J35" s="23"/>
       <c r="K35" s="23"/>
     </row>
     <row r="36" spans="1:11" s="6" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
-      <c r="B36" s="62" t="s">
+      <c r="B36" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="64"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="62"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
@@ -1818,15 +1821,15 @@
     </row>
     <row r="39" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
-      <c r="B39" s="65" t="s">
+      <c r="B39" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="66"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="66"/>
-      <c r="G39" s="66"/>
-      <c r="H39" s="67"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="75"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
@@ -1848,30 +1851,30 @@
       <c r="A41" s="21">
         <v>7</v>
       </c>
-      <c r="B41" s="54" t="s">
+      <c r="B41" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="54"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="54"/>
-      <c r="H41" s="54"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
     </row>
     <row r="42" spans="1:11" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
-      <c r="B42" s="62" t="s">
+      <c r="B42" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="64"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="62"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
@@ -1893,30 +1896,30 @@
       <c r="A44" s="21">
         <v>8</v>
       </c>
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="54"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="54"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
     </row>
     <row r="45" spans="1:11" s="6" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
-      <c r="B45" s="62" t="s">
+      <c r="B45" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
-      <c r="G45" s="63"/>
-      <c r="H45" s="64"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="62"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
@@ -2070,13 +2073,13 @@
       <c r="A56" s="13"/>
       <c r="B56" s="12"/>
       <c r="C56" s="20"/>
-      <c r="D56" s="69" t="s">
+      <c r="D56" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="E56" s="70"/>
-      <c r="F56" s="70"/>
-      <c r="G56" s="70"/>
-      <c r="H56" s="71"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="48"/>
     </row>
     <row r="57" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
@@ -2092,27 +2095,27 @@
       <c r="A58" s="21">
         <v>10</v>
       </c>
-      <c r="B58" s="54" t="s">
+      <c r="B58" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="54"/>
-      <c r="D58" s="54"/>
-      <c r="E58" s="54"/>
-      <c r="F58" s="54"/>
-      <c r="G58" s="54"/>
-      <c r="H58" s="54"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63"/>
+      <c r="E58" s="63"/>
+      <c r="F58" s="63"/>
+      <c r="G58" s="63"/>
+      <c r="H58" s="63"/>
     </row>
     <row r="59" spans="1:8" s="6" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
-      <c r="B59" s="62" t="s">
+      <c r="B59" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="63"/>
-      <c r="D59" s="63"/>
-      <c r="E59" s="63"/>
-      <c r="F59" s="63"/>
-      <c r="G59" s="63"/>
-      <c r="H59" s="64"/>
+      <c r="C59" s="61"/>
+      <c r="D59" s="61"/>
+      <c r="E59" s="61"/>
+      <c r="F59" s="61"/>
+      <c r="G59" s="61"/>
+      <c r="H59" s="62"/>
     </row>
     <row r="60" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
@@ -2128,27 +2131,27 @@
       <c r="A61" s="21">
         <v>11</v>
       </c>
-      <c r="B61" s="54" t="s">
+      <c r="B61" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="54"/>
-      <c r="D61" s="54"/>
-      <c r="E61" s="54"/>
-      <c r="F61" s="54"/>
-      <c r="G61" s="54"/>
-      <c r="H61" s="54"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="63"/>
+      <c r="F61" s="63"/>
+      <c r="G61" s="63"/>
+      <c r="H61" s="63"/>
     </row>
     <row r="62" spans="1:8" s="6" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
-      <c r="B62" s="62" t="s">
+      <c r="B62" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="63"/>
-      <c r="D62" s="63"/>
-      <c r="E62" s="63"/>
-      <c r="F62" s="63"/>
-      <c r="G62" s="63"/>
-      <c r="H62" s="64"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="61"/>
+      <c r="F62" s="61"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="62"/>
     </row>
     <row r="63" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
@@ -2164,15 +2167,15 @@
       <c r="A64" s="36">
         <v>12</v>
       </c>
-      <c r="B64" s="54" t="s">
+      <c r="B64" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="54"/>
-      <c r="D64" s="54"/>
-      <c r="E64" s="54"/>
-      <c r="F64" s="54"/>
-      <c r="G64" s="54"/>
-      <c r="H64" s="54"/>
+      <c r="C64" s="63"/>
+      <c r="D64" s="63"/>
+      <c r="E64" s="63"/>
+      <c r="F64" s="63"/>
+      <c r="G64" s="63"/>
+      <c r="H64" s="63"/>
     </row>
     <row r="65" spans="1:8" s="6" customFormat="1" ht="86.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
@@ -2181,14 +2184,14 @@
       <c r="B65" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="72" t="s">
+      <c r="C65" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="72"/>
-      <c r="H65" s="72"/>
+      <c r="D65" s="64"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="64"/>
+      <c r="H65" s="64"/>
     </row>
     <row r="66" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
@@ -2197,14 +2200,14 @@
       <c r="B66" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="68" t="s">
+      <c r="C66" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="D66" s="68"/>
-      <c r="E66" s="68"/>
-      <c r="F66" s="68"/>
-      <c r="G66" s="68"/>
-      <c r="H66" s="68"/>
+      <c r="D66" s="55"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="55"/>
+      <c r="G66" s="55"/>
+      <c r="H66" s="55"/>
     </row>
     <row r="67" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
@@ -2213,14 +2216,14 @@
       <c r="B67" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C67" s="68" t="s">
+      <c r="C67" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="D67" s="68"/>
-      <c r="E67" s="68"/>
-      <c r="F67" s="68"/>
-      <c r="G67" s="68"/>
-      <c r="H67" s="68"/>
+      <c r="D67" s="55"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="55"/>
+      <c r="G67" s="55"/>
+      <c r="H67" s="55"/>
     </row>
     <row r="68" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
@@ -2229,14 +2232,14 @@
       <c r="B68" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="D68" s="68"/>
-      <c r="E68" s="68"/>
-      <c r="F68" s="68"/>
-      <c r="G68" s="68"/>
-      <c r="H68" s="68"/>
+      <c r="D68" s="55"/>
+      <c r="E68" s="55"/>
+      <c r="F68" s="55"/>
+      <c r="G68" s="55"/>
+      <c r="H68" s="55"/>
     </row>
     <row r="69" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
@@ -2245,14 +2248,14 @@
       <c r="B69" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="C69" s="68" t="s">
+      <c r="C69" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="D69" s="68"/>
-      <c r="E69" s="68"/>
-      <c r="F69" s="68"/>
-      <c r="G69" s="68"/>
-      <c r="H69" s="68"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="55"/>
+      <c r="G69" s="55"/>
+      <c r="H69" s="55"/>
     </row>
     <row r="70" spans="1:8" s="6" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
@@ -2261,14 +2264,14 @@
       <c r="B70" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="C70" s="74" t="s">
+      <c r="C70" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="D70" s="75"/>
-      <c r="E70" s="75"/>
-      <c r="F70" s="75"/>
-      <c r="G70" s="75"/>
-      <c r="H70" s="76"/>
+      <c r="D70" s="58"/>
+      <c r="E70" s="58"/>
+      <c r="F70" s="58"/>
+      <c r="G70" s="58"/>
+      <c r="H70" s="59"/>
     </row>
     <row r="71" spans="1:8" s="6" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
@@ -2277,14 +2280,14 @@
       <c r="B71" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="C71" s="68" t="s">
+      <c r="C71" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="D71" s="68"/>
-      <c r="E71" s="68"/>
-      <c r="F71" s="68"/>
-      <c r="G71" s="68"/>
-      <c r="H71" s="68"/>
+      <c r="D71" s="55"/>
+      <c r="E71" s="55"/>
+      <c r="F71" s="55"/>
+      <c r="G71" s="55"/>
+      <c r="H71" s="55"/>
     </row>
     <row r="72" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
@@ -2293,14 +2296,14 @@
       <c r="B72" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C72" s="68" t="s">
+      <c r="C72" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="D72" s="68"/>
-      <c r="E72" s="68"/>
-      <c r="F72" s="68"/>
-      <c r="G72" s="68"/>
-      <c r="H72" s="68"/>
+      <c r="D72" s="55"/>
+      <c r="E72" s="55"/>
+      <c r="F72" s="55"/>
+      <c r="G72" s="55"/>
+      <c r="H72" s="55"/>
     </row>
     <row r="73" spans="1:8" s="6" customFormat="1" ht="66.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
@@ -2309,14 +2312,14 @@
       <c r="B73" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="D73" s="68"/>
-      <c r="E73" s="68"/>
-      <c r="F73" s="68"/>
-      <c r="G73" s="68"/>
-      <c r="H73" s="68"/>
+      <c r="D73" s="55"/>
+      <c r="E73" s="55"/>
+      <c r="F73" s="55"/>
+      <c r="G73" s="55"/>
+      <c r="H73" s="55"/>
     </row>
     <row r="74" spans="1:8" s="6" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
@@ -2325,14 +2328,14 @@
       <c r="B74" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="C74" s="68" t="s">
+      <c r="C74" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="D74" s="68"/>
-      <c r="E74" s="68"/>
-      <c r="F74" s="68"/>
-      <c r="G74" s="68"/>
-      <c r="H74" s="68"/>
+      <c r="D74" s="55"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="55"/>
+      <c r="G74" s="55"/>
+      <c r="H74" s="55"/>
     </row>
     <row r="75" spans="1:8" s="6" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
@@ -2341,14 +2344,14 @@
       <c r="B75" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="C75" s="68" t="s">
+      <c r="C75" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="D75" s="68"/>
-      <c r="E75" s="68"/>
-      <c r="F75" s="68"/>
-      <c r="G75" s="68"/>
-      <c r="H75" s="68"/>
+      <c r="D75" s="55"/>
+      <c r="E75" s="55"/>
+      <c r="F75" s="55"/>
+      <c r="G75" s="55"/>
+      <c r="H75" s="55"/>
     </row>
     <row r="76" spans="1:8" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
@@ -2357,14 +2360,14 @@
       <c r="B76" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="C76" s="68" t="s">
+      <c r="C76" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="D76" s="68"/>
-      <c r="E76" s="68"/>
-      <c r="F76" s="68"/>
-      <c r="G76" s="68"/>
-      <c r="H76" s="68"/>
+      <c r="D76" s="55"/>
+      <c r="E76" s="55"/>
+      <c r="F76" s="55"/>
+      <c r="G76" s="55"/>
+      <c r="H76" s="55"/>
     </row>
     <row r="77" spans="1:8" s="6" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
@@ -2373,14 +2376,14 @@
       <c r="B77" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="C77" s="68" t="s">
+      <c r="C77" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="D77" s="68"/>
-      <c r="E77" s="68"/>
-      <c r="F77" s="68"/>
-      <c r="G77" s="68"/>
-      <c r="H77" s="68"/>
+      <c r="D77" s="55"/>
+      <c r="E77" s="55"/>
+      <c r="F77" s="55"/>
+      <c r="G77" s="55"/>
+      <c r="H77" s="55"/>
     </row>
     <row r="78" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
@@ -2389,14 +2392,14 @@
       <c r="B78" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="D78" s="68"/>
-      <c r="E78" s="68"/>
-      <c r="F78" s="68"/>
-      <c r="G78" s="68"/>
-      <c r="H78" s="68"/>
+      <c r="D78" s="55"/>
+      <c r="E78" s="55"/>
+      <c r="F78" s="55"/>
+      <c r="G78" s="55"/>
+      <c r="H78" s="55"/>
     </row>
     <row r="79" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="42"/>
@@ -2412,15 +2415,15 @@
       <c r="A80" s="21">
         <v>13</v>
       </c>
-      <c r="B80" s="73" t="s">
+      <c r="B80" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="C80" s="73"/>
-      <c r="D80" s="73"/>
-      <c r="E80" s="73"/>
-      <c r="F80" s="73"/>
-      <c r="G80" s="73"/>
-      <c r="H80" s="73"/>
+      <c r="C80" s="56"/>
+      <c r="D80" s="56"/>
+      <c r="E80" s="56"/>
+      <c r="F80" s="56"/>
+      <c r="G80" s="56"/>
+      <c r="H80" s="56"/>
     </row>
     <row r="81" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
@@ -2429,14 +2432,14 @@
       <c r="B81" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="C81" s="68" t="s">
+      <c r="C81" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="D81" s="68"/>
-      <c r="E81" s="68"/>
-      <c r="F81" s="68"/>
-      <c r="G81" s="68"/>
-      <c r="H81" s="68"/>
+      <c r="D81" s="55"/>
+      <c r="E81" s="55"/>
+      <c r="F81" s="55"/>
+      <c r="G81" s="55"/>
+      <c r="H81" s="55"/>
     </row>
     <row r="82" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
@@ -2445,14 +2448,14 @@
       <c r="B82" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="C82" s="68" t="s">
+      <c r="C82" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="D82" s="68"/>
-      <c r="E82" s="68"/>
-      <c r="F82" s="68"/>
-      <c r="G82" s="68"/>
-      <c r="H82" s="68"/>
+      <c r="D82" s="55"/>
+      <c r="E82" s="55"/>
+      <c r="F82" s="55"/>
+      <c r="G82" s="55"/>
+      <c r="H82" s="55"/>
     </row>
     <row r="83" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="16" t="s">
@@ -2461,14 +2464,14 @@
       <c r="B83" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="C83" s="68" t="s">
+      <c r="C83" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="D83" s="68"/>
-      <c r="E83" s="68"/>
-      <c r="F83" s="68"/>
-      <c r="G83" s="68"/>
-      <c r="H83" s="68"/>
+      <c r="D83" s="55"/>
+      <c r="E83" s="55"/>
+      <c r="F83" s="55"/>
+      <c r="G83" s="55"/>
+      <c r="H83" s="55"/>
     </row>
     <row r="84" spans="1:8" s="6" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
@@ -2477,14 +2480,14 @@
       <c r="B84" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="C84" s="68" t="s">
+      <c r="C84" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="D84" s="68"/>
-      <c r="E84" s="68"/>
-      <c r="F84" s="68"/>
-      <c r="G84" s="68"/>
-      <c r="H84" s="68"/>
+      <c r="D84" s="55"/>
+      <c r="E84" s="55"/>
+      <c r="F84" s="55"/>
+      <c r="G84" s="55"/>
+      <c r="H84" s="55"/>
     </row>
     <row r="85" spans="1:8" s="6" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
@@ -2493,14 +2496,14 @@
       <c r="B85" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C85" s="68" t="s">
+      <c r="C85" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="D85" s="68"/>
-      <c r="E85" s="68"/>
-      <c r="F85" s="68"/>
-      <c r="G85" s="68"/>
-      <c r="H85" s="68"/>
+      <c r="D85" s="55"/>
+      <c r="E85" s="55"/>
+      <c r="F85" s="55"/>
+      <c r="G85" s="55"/>
+      <c r="H85" s="55"/>
     </row>
     <row r="86" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="16" t="s">
@@ -2509,14 +2512,14 @@
       <c r="B86" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="C86" s="68" t="s">
+      <c r="C86" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="D86" s="68"/>
-      <c r="E86" s="68"/>
-      <c r="F86" s="68"/>
-      <c r="G86" s="68"/>
-      <c r="H86" s="68"/>
+      <c r="D86" s="55"/>
+      <c r="E86" s="55"/>
+      <c r="F86" s="55"/>
+      <c r="G86" s="55"/>
+      <c r="H86" s="55"/>
     </row>
     <row r="87" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="16" t="s">
@@ -2525,14 +2528,14 @@
       <c r="B87" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="C87" s="68" t="s">
+      <c r="C87" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="D87" s="68"/>
-      <c r="E87" s="68"/>
-      <c r="F87" s="68"/>
-      <c r="G87" s="68"/>
-      <c r="H87" s="68"/>
+      <c r="D87" s="55"/>
+      <c r="E87" s="55"/>
+      <c r="F87" s="55"/>
+      <c r="G87" s="55"/>
+      <c r="H87" s="55"/>
     </row>
     <row r="88" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="16" t="s">
@@ -2541,14 +2544,14 @@
       <c r="B88" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C88" s="68" t="s">
+      <c r="C88" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="D88" s="68"/>
-      <c r="E88" s="68"/>
-      <c r="F88" s="68"/>
-      <c r="G88" s="68"/>
-      <c r="H88" s="68"/>
+      <c r="D88" s="55"/>
+      <c r="E88" s="55"/>
+      <c r="F88" s="55"/>
+      <c r="G88" s="55"/>
+      <c r="H88" s="55"/>
     </row>
     <row r="89" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="16" t="s">
@@ -2557,14 +2560,14 @@
       <c r="B89" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="C89" s="68" t="s">
+      <c r="C89" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="D89" s="68"/>
-      <c r="E89" s="68"/>
-      <c r="F89" s="68"/>
-      <c r="G89" s="68"/>
-      <c r="H89" s="68"/>
+      <c r="D89" s="55"/>
+      <c r="E89" s="55"/>
+      <c r="F89" s="55"/>
+      <c r="G89" s="55"/>
+      <c r="H89" s="55"/>
     </row>
     <row r="90" spans="1:8" s="6" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="16" t="s">
@@ -2573,14 +2576,14 @@
       <c r="B90" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="C90" s="68" t="s">
+      <c r="C90" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="D90" s="68"/>
-      <c r="E90" s="68"/>
-      <c r="F90" s="68"/>
-      <c r="G90" s="68"/>
-      <c r="H90" s="68"/>
+      <c r="D90" s="55"/>
+      <c r="E90" s="55"/>
+      <c r="F90" s="55"/>
+      <c r="G90" s="55"/>
+      <c r="H90" s="55"/>
     </row>
     <row r="91" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="16" t="s">
@@ -2589,12 +2592,14 @@
       <c r="B91" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C91" s="68"/>
-      <c r="D91" s="68"/>
-      <c r="E91" s="68"/>
-      <c r="F91" s="68"/>
-      <c r="G91" s="68"/>
-      <c r="H91" s="68"/>
+      <c r="C91" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="D91" s="55"/>
+      <c r="E91" s="55"/>
+      <c r="F91" s="55"/>
+      <c r="G91" s="55"/>
+      <c r="H91" s="55"/>
     </row>
     <row r="92" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="15"/>
@@ -2610,27 +2615,27 @@
       <c r="A93" s="21">
         <v>14</v>
       </c>
-      <c r="B93" s="77" t="s">
+      <c r="B93" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="C93" s="77"/>
-      <c r="D93" s="77"/>
-      <c r="E93" s="77"/>
-      <c r="F93" s="77"/>
-      <c r="G93" s="77"/>
-      <c r="H93" s="77"/>
+      <c r="C93" s="54"/>
+      <c r="D93" s="54"/>
+      <c r="E93" s="54"/>
+      <c r="F93" s="54"/>
+      <c r="G93" s="54"/>
+      <c r="H93" s="54"/>
     </row>
     <row r="94" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
-      <c r="B94" s="69" t="s">
+      <c r="B94" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C94" s="70"/>
-      <c r="D94" s="70"/>
-      <c r="E94" s="70"/>
-      <c r="F94" s="70"/>
-      <c r="G94" s="70"/>
-      <c r="H94" s="71"/>
+      <c r="C94" s="47"/>
+      <c r="D94" s="47"/>
+      <c r="E94" s="47"/>
+      <c r="F94" s="47"/>
+      <c r="G94" s="47"/>
+      <c r="H94" s="48"/>
     </row>
     <row r="95" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="15"/>
@@ -2646,27 +2651,27 @@
       <c r="A96" s="45">
         <v>15</v>
       </c>
-      <c r="B96" s="78" t="s">
+      <c r="B96" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="C96" s="78"/>
-      <c r="D96" s="78"/>
-      <c r="E96" s="78"/>
-      <c r="F96" s="78"/>
-      <c r="G96" s="78"/>
-      <c r="H96" s="78"/>
+      <c r="C96" s="49"/>
+      <c r="D96" s="49"/>
+      <c r="E96" s="49"/>
+      <c r="F96" s="49"/>
+      <c r="G96" s="49"/>
+      <c r="H96" s="49"/>
     </row>
     <row r="97" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
-      <c r="B97" s="69" t="s">
+      <c r="B97" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C97" s="70"/>
-      <c r="D97" s="70"/>
-      <c r="E97" s="70"/>
-      <c r="F97" s="70"/>
-      <c r="G97" s="70"/>
-      <c r="H97" s="71"/>
+      <c r="C97" s="47"/>
+      <c r="D97" s="47"/>
+      <c r="E97" s="47"/>
+      <c r="F97" s="47"/>
+      <c r="G97" s="47"/>
+      <c r="H97" s="48"/>
     </row>
     <row r="98" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="15"/>
@@ -2682,27 +2687,27 @@
       <c r="A99" s="21">
         <v>16</v>
       </c>
-      <c r="B99" s="79" t="s">
+      <c r="B99" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="C99" s="79"/>
-      <c r="D99" s="79"/>
-      <c r="E99" s="79"/>
-      <c r="F99" s="79"/>
-      <c r="G99" s="79"/>
-      <c r="H99" s="79"/>
+      <c r="C99" s="50"/>
+      <c r="D99" s="50"/>
+      <c r="E99" s="50"/>
+      <c r="F99" s="50"/>
+      <c r="G99" s="50"/>
+      <c r="H99" s="50"/>
     </row>
     <row r="100" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
-      <c r="B100" s="80" t="s">
+      <c r="B100" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="C100" s="81"/>
-      <c r="D100" s="81"/>
-      <c r="E100" s="81"/>
-      <c r="F100" s="81"/>
-      <c r="G100" s="81"/>
-      <c r="H100" s="82"/>
+      <c r="C100" s="52"/>
+      <c r="D100" s="52"/>
+      <c r="E100" s="52"/>
+      <c r="F100" s="52"/>
+      <c r="G100" s="52"/>
+      <c r="H100" s="53"/>
     </row>
     <row r="101" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="15"/>
@@ -2716,59 +2721,6 @@
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="B94:H94"/>
-    <mergeCell ref="B96:H96"/>
-    <mergeCell ref="B97:H97"/>
-    <mergeCell ref="B99:H99"/>
-    <mergeCell ref="B100:H100"/>
-    <mergeCell ref="B93:H93"/>
-    <mergeCell ref="C81:H81"/>
-    <mergeCell ref="C82:H82"/>
-    <mergeCell ref="C83:H83"/>
-    <mergeCell ref="C84:H84"/>
-    <mergeCell ref="C85:H85"/>
-    <mergeCell ref="C86:H86"/>
-    <mergeCell ref="C87:H87"/>
-    <mergeCell ref="C88:H88"/>
-    <mergeCell ref="C89:H89"/>
-    <mergeCell ref="C90:H90"/>
-    <mergeCell ref="C91:H91"/>
-    <mergeCell ref="B80:H80"/>
-    <mergeCell ref="C68:H68"/>
-    <mergeCell ref="C69:H69"/>
-    <mergeCell ref="C71:H71"/>
-    <mergeCell ref="C72:H72"/>
-    <mergeCell ref="C73:H73"/>
-    <mergeCell ref="C74:H74"/>
-    <mergeCell ref="C75:H75"/>
-    <mergeCell ref="C76:H76"/>
-    <mergeCell ref="C77:H77"/>
-    <mergeCell ref="C78:H78"/>
-    <mergeCell ref="C70:H70"/>
-    <mergeCell ref="C67:H67"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="D56:H56"/>
-    <mergeCell ref="B58:H58"/>
-    <mergeCell ref="B59:H59"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="B62:H62"/>
-    <mergeCell ref="B64:H64"/>
-    <mergeCell ref="C65:H65"/>
-    <mergeCell ref="C66:H66"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="B39:H39"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="A3:H3"/>
@@ -2782,6 +2734,59 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="C67:H67"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="D56:H56"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B62:H62"/>
+    <mergeCell ref="B64:H64"/>
+    <mergeCell ref="C65:H65"/>
+    <mergeCell ref="C66:H66"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="C68:H68"/>
+    <mergeCell ref="C69:H69"/>
+    <mergeCell ref="C71:H71"/>
+    <mergeCell ref="C72:H72"/>
+    <mergeCell ref="C73:H73"/>
+    <mergeCell ref="C74:H74"/>
+    <mergeCell ref="C75:H75"/>
+    <mergeCell ref="C76:H76"/>
+    <mergeCell ref="C77:H77"/>
+    <mergeCell ref="C78:H78"/>
+    <mergeCell ref="C70:H70"/>
+    <mergeCell ref="B93:H93"/>
+    <mergeCell ref="C81:H81"/>
+    <mergeCell ref="C82:H82"/>
+    <mergeCell ref="C83:H83"/>
+    <mergeCell ref="C84:H84"/>
+    <mergeCell ref="C85:H85"/>
+    <mergeCell ref="C86:H86"/>
+    <mergeCell ref="C87:H87"/>
+    <mergeCell ref="C88:H88"/>
+    <mergeCell ref="C89:H89"/>
+    <mergeCell ref="C90:H90"/>
+    <mergeCell ref="C91:H91"/>
+    <mergeCell ref="B94:H94"/>
+    <mergeCell ref="B96:H96"/>
+    <mergeCell ref="B97:H97"/>
+    <mergeCell ref="B99:H99"/>
+    <mergeCell ref="B100:H100"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
minor chnages made now the loop cathes files independent to their names
</commit_message>
<xml_diff>
--- a/SummerWork/All_Reports/Adrian_SD_61_2017-2018_Outdoor_School_Report.xlsx
+++ b/SummerWork/All_Reports/Adrian_SD_61_2017-2018_Outdoor_School_Report.xlsx
@@ -24,7 +24,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Adrian School District #61'!$A$1:$H$101</definedName>
     <definedName name="Provider">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="132">
   <si>
     <t>2017-2018 Outdoor School - Reporting Form</t>
   </si>
@@ -456,9 +456,6 @@
   </si>
   <si>
     <t>In the past, the teacher representing the class that is attending has budjeted for part of Outdoor School with the rest of the funding coming through fundraisers and individual donations.</t>
-  </si>
-  <si>
-    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -807,6 +804,75 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -816,6 +882,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -830,93 +914,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1211,8 +1208,8 @@
   </sheetPr>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="63" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91:H91"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="63" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81:H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1229,15 +1226,15 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -1254,28 +1251,28 @@
       <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
@@ -1291,15 +1288,15 @@
       <c r="A6" s="14">
         <v>1</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
@@ -1315,69 +1312,69 @@
       <c r="A8" s="16">
         <v>2</v>
       </c>
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="80"/>
+      <c r="D9" s="51"/>
       <c r="E9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="79" t="s">
+      <c r="F9" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="81"/>
-      <c r="H9" s="80"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="51"/>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="82" t="s">
+      <c r="C10" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="80"/>
+      <c r="D10" s="51"/>
       <c r="E10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="82" t="s">
+      <c r="F10" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="81"/>
-      <c r="H10" s="80"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="51"/>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="80"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="79" t="s">
+      <c r="F11" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="81"/>
-      <c r="H11" s="80"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="51"/>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
@@ -1407,66 +1404,66 @@
       <c r="A14" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="76" t="s">
+      <c r="B14" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
     </row>
     <row r="17" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
     </row>
     <row r="18" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="68"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="57"/>
       <c r="G18" s="22">
         <v>5</v>
       </c>
@@ -1477,13 +1474,13 @@
     </row>
     <row r="19" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="70"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="59"/>
       <c r="G19" s="22">
         <v>3</v>
       </c>
@@ -1494,13 +1491,13 @@
     </row>
     <row r="20" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="70"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="59"/>
       <c r="G20" s="22">
         <v>4</v>
       </c>
@@ -1511,13 +1508,13 @@
     </row>
     <row r="21" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
-      <c r="B21" s="71" t="s">
+      <c r="B21" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="70"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="59"/>
       <c r="G21" s="22">
         <v>5</v>
       </c>
@@ -1528,13 +1525,13 @@
     </row>
     <row r="22" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="70"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="59"/>
       <c r="G22" s="22">
         <v>5</v>
       </c>
@@ -1575,15 +1572,15 @@
     </row>
     <row r="25" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
-      <c r="B25" s="65" t="s">
+      <c r="B25" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
@@ -1761,30 +1758,30 @@
       <c r="A35" s="21">
         <v>5</v>
       </c>
-      <c r="B35" s="72" t="s">
+      <c r="B35" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="72"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
       <c r="I35" s="23"/>
       <c r="J35" s="23"/>
       <c r="K35" s="23"/>
     </row>
     <row r="36" spans="1:11" s="6" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
-      <c r="B36" s="60" t="s">
+      <c r="B36" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="61"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="61"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="62"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="63"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="64"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
@@ -1821,15 +1818,15 @@
     </row>
     <row r="39" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
-      <c r="B39" s="73" t="s">
+      <c r="B39" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="74"/>
-      <c r="D39" s="74"/>
-      <c r="E39" s="74"/>
-      <c r="F39" s="74"/>
-      <c r="G39" s="74"/>
-      <c r="H39" s="75"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="67"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
@@ -1851,30 +1848,30 @@
       <c r="A41" s="21">
         <v>7</v>
       </c>
-      <c r="B41" s="63" t="s">
+      <c r="B41" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="63"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="63"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
     </row>
     <row r="42" spans="1:11" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
-      <c r="B42" s="60" t="s">
+      <c r="B42" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="62"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="63"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="64"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
@@ -1896,30 +1893,30 @@
       <c r="A44" s="21">
         <v>8</v>
       </c>
-      <c r="B44" s="63" t="s">
+      <c r="B44" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="63"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="63"/>
-      <c r="G44" s="63"/>
-      <c r="H44" s="63"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
     </row>
     <row r="45" spans="1:11" s="6" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
-      <c r="B45" s="60" t="s">
+      <c r="B45" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="62"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="63"/>
+      <c r="F45" s="63"/>
+      <c r="G45" s="63"/>
+      <c r="H45" s="64"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
@@ -2073,13 +2070,13 @@
       <c r="A56" s="13"/>
       <c r="B56" s="12"/>
       <c r="C56" s="20"/>
-      <c r="D56" s="46" t="s">
+      <c r="D56" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="E56" s="47"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="48"/>
+      <c r="E56" s="70"/>
+      <c r="F56" s="70"/>
+      <c r="G56" s="70"/>
+      <c r="H56" s="71"/>
     </row>
     <row r="57" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
@@ -2095,27 +2092,27 @@
       <c r="A58" s="21">
         <v>10</v>
       </c>
-      <c r="B58" s="63" t="s">
+      <c r="B58" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="63"/>
-      <c r="D58" s="63"/>
-      <c r="E58" s="63"/>
-      <c r="F58" s="63"/>
-      <c r="G58" s="63"/>
-      <c r="H58" s="63"/>
+      <c r="C58" s="54"/>
+      <c r="D58" s="54"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="54"/>
+      <c r="G58" s="54"/>
+      <c r="H58" s="54"/>
     </row>
     <row r="59" spans="1:8" s="6" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
-      <c r="B59" s="60" t="s">
+      <c r="B59" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="61"/>
-      <c r="D59" s="61"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="61"/>
-      <c r="G59" s="61"/>
-      <c r="H59" s="62"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="63"/>
+      <c r="F59" s="63"/>
+      <c r="G59" s="63"/>
+      <c r="H59" s="64"/>
     </row>
     <row r="60" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
@@ -2131,27 +2128,27 @@
       <c r="A61" s="21">
         <v>11</v>
       </c>
-      <c r="B61" s="63" t="s">
+      <c r="B61" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="63"/>
-      <c r="D61" s="63"/>
-      <c r="E61" s="63"/>
-      <c r="F61" s="63"/>
-      <c r="G61" s="63"/>
-      <c r="H61" s="63"/>
+      <c r="C61" s="54"/>
+      <c r="D61" s="54"/>
+      <c r="E61" s="54"/>
+      <c r="F61" s="54"/>
+      <c r="G61" s="54"/>
+      <c r="H61" s="54"/>
     </row>
     <row r="62" spans="1:8" s="6" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
-      <c r="B62" s="60" t="s">
+      <c r="B62" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="61"/>
-      <c r="D62" s="61"/>
-      <c r="E62" s="61"/>
-      <c r="F62" s="61"/>
-      <c r="G62" s="61"/>
-      <c r="H62" s="62"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="63"/>
+      <c r="E62" s="63"/>
+      <c r="F62" s="63"/>
+      <c r="G62" s="63"/>
+      <c r="H62" s="64"/>
     </row>
     <row r="63" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
@@ -2167,15 +2164,15 @@
       <c r="A64" s="36">
         <v>12</v>
       </c>
-      <c r="B64" s="63" t="s">
+      <c r="B64" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="63"/>
-      <c r="D64" s="63"/>
-      <c r="E64" s="63"/>
-      <c r="F64" s="63"/>
-      <c r="G64" s="63"/>
-      <c r="H64" s="63"/>
+      <c r="C64" s="54"/>
+      <c r="D64" s="54"/>
+      <c r="E64" s="54"/>
+      <c r="F64" s="54"/>
+      <c r="G64" s="54"/>
+      <c r="H64" s="54"/>
     </row>
     <row r="65" spans="1:8" s="6" customFormat="1" ht="86.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
@@ -2184,14 +2181,14 @@
       <c r="B65" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="64" t="s">
+      <c r="C65" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="D65" s="64"/>
-      <c r="E65" s="64"/>
-      <c r="F65" s="64"/>
-      <c r="G65" s="64"/>
-      <c r="H65" s="64"/>
+      <c r="D65" s="72"/>
+      <c r="E65" s="72"/>
+      <c r="F65" s="72"/>
+      <c r="G65" s="72"/>
+      <c r="H65" s="72"/>
     </row>
     <row r="66" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
@@ -2200,14 +2197,14 @@
       <c r="B66" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="55" t="s">
+      <c r="C66" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="D66" s="55"/>
-      <c r="E66" s="55"/>
-      <c r="F66" s="55"/>
-      <c r="G66" s="55"/>
-      <c r="H66" s="55"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="68"/>
+      <c r="H66" s="68"/>
     </row>
     <row r="67" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
@@ -2216,14 +2213,14 @@
       <c r="B67" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C67" s="55" t="s">
+      <c r="C67" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="D67" s="55"/>
-      <c r="E67" s="55"/>
-      <c r="F67" s="55"/>
-      <c r="G67" s="55"/>
-      <c r="H67" s="55"/>
+      <c r="D67" s="68"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="68"/>
+      <c r="G67" s="68"/>
+      <c r="H67" s="68"/>
     </row>
     <row r="68" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
@@ -2232,14 +2229,14 @@
       <c r="B68" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C68" s="55" t="s">
+      <c r="C68" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="D68" s="55"/>
-      <c r="E68" s="55"/>
-      <c r="F68" s="55"/>
-      <c r="G68" s="55"/>
-      <c r="H68" s="55"/>
+      <c r="D68" s="68"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
+      <c r="G68" s="68"/>
+      <c r="H68" s="68"/>
     </row>
     <row r="69" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
@@ -2248,14 +2245,14 @@
       <c r="B69" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="C69" s="55" t="s">
+      <c r="C69" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="D69" s="55"/>
-      <c r="E69" s="55"/>
-      <c r="F69" s="55"/>
-      <c r="G69" s="55"/>
-      <c r="H69" s="55"/>
+      <c r="D69" s="68"/>
+      <c r="E69" s="68"/>
+      <c r="F69" s="68"/>
+      <c r="G69" s="68"/>
+      <c r="H69" s="68"/>
     </row>
     <row r="70" spans="1:8" s="6" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
@@ -2264,14 +2261,14 @@
       <c r="B70" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="C70" s="57" t="s">
+      <c r="C70" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
-      <c r="F70" s="58"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="59"/>
+      <c r="D70" s="75"/>
+      <c r="E70" s="75"/>
+      <c r="F70" s="75"/>
+      <c r="G70" s="75"/>
+      <c r="H70" s="76"/>
     </row>
     <row r="71" spans="1:8" s="6" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
@@ -2280,14 +2277,14 @@
       <c r="B71" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="C71" s="55" t="s">
+      <c r="C71" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="D71" s="55"/>
-      <c r="E71" s="55"/>
-      <c r="F71" s="55"/>
-      <c r="G71" s="55"/>
-      <c r="H71" s="55"/>
+      <c r="D71" s="68"/>
+      <c r="E71" s="68"/>
+      <c r="F71" s="68"/>
+      <c r="G71" s="68"/>
+      <c r="H71" s="68"/>
     </row>
     <row r="72" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
@@ -2296,14 +2293,14 @@
       <c r="B72" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C72" s="55" t="s">
+      <c r="C72" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="D72" s="55"/>
-      <c r="E72" s="55"/>
-      <c r="F72" s="55"/>
-      <c r="G72" s="55"/>
-      <c r="H72" s="55"/>
+      <c r="D72" s="68"/>
+      <c r="E72" s="68"/>
+      <c r="F72" s="68"/>
+      <c r="G72" s="68"/>
+      <c r="H72" s="68"/>
     </row>
     <row r="73" spans="1:8" s="6" customFormat="1" ht="66.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
@@ -2312,14 +2309,14 @@
       <c r="B73" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="C73" s="55" t="s">
+      <c r="C73" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="D73" s="55"/>
-      <c r="E73" s="55"/>
-      <c r="F73" s="55"/>
-      <c r="G73" s="55"/>
-      <c r="H73" s="55"/>
+      <c r="D73" s="68"/>
+      <c r="E73" s="68"/>
+      <c r="F73" s="68"/>
+      <c r="G73" s="68"/>
+      <c r="H73" s="68"/>
     </row>
     <row r="74" spans="1:8" s="6" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
@@ -2328,14 +2325,14 @@
       <c r="B74" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="C74" s="55" t="s">
+      <c r="C74" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="D74" s="55"/>
-      <c r="E74" s="55"/>
-      <c r="F74" s="55"/>
-      <c r="G74" s="55"/>
-      <c r="H74" s="55"/>
+      <c r="D74" s="68"/>
+      <c r="E74" s="68"/>
+      <c r="F74" s="68"/>
+      <c r="G74" s="68"/>
+      <c r="H74" s="68"/>
     </row>
     <row r="75" spans="1:8" s="6" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
@@ -2344,14 +2341,14 @@
       <c r="B75" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="C75" s="55" t="s">
+      <c r="C75" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="D75" s="55"/>
-      <c r="E75" s="55"/>
-      <c r="F75" s="55"/>
-      <c r="G75" s="55"/>
-      <c r="H75" s="55"/>
+      <c r="D75" s="68"/>
+      <c r="E75" s="68"/>
+      <c r="F75" s="68"/>
+      <c r="G75" s="68"/>
+      <c r="H75" s="68"/>
     </row>
     <row r="76" spans="1:8" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
@@ -2360,14 +2357,14 @@
       <c r="B76" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="C76" s="55" t="s">
+      <c r="C76" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="D76" s="55"/>
-      <c r="E76" s="55"/>
-      <c r="F76" s="55"/>
-      <c r="G76" s="55"/>
-      <c r="H76" s="55"/>
+      <c r="D76" s="68"/>
+      <c r="E76" s="68"/>
+      <c r="F76" s="68"/>
+      <c r="G76" s="68"/>
+      <c r="H76" s="68"/>
     </row>
     <row r="77" spans="1:8" s="6" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
@@ -2376,14 +2373,14 @@
       <c r="B77" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="C77" s="55" t="s">
+      <c r="C77" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="D77" s="55"/>
-      <c r="E77" s="55"/>
-      <c r="F77" s="55"/>
-      <c r="G77" s="55"/>
-      <c r="H77" s="55"/>
+      <c r="D77" s="68"/>
+      <c r="E77" s="68"/>
+      <c r="F77" s="68"/>
+      <c r="G77" s="68"/>
+      <c r="H77" s="68"/>
     </row>
     <row r="78" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
@@ -2392,14 +2389,14 @@
       <c r="B78" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="C78" s="55" t="s">
+      <c r="C78" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="D78" s="55"/>
-      <c r="E78" s="55"/>
-      <c r="F78" s="55"/>
-      <c r="G78" s="55"/>
-      <c r="H78" s="55"/>
+      <c r="D78" s="68"/>
+      <c r="E78" s="68"/>
+      <c r="F78" s="68"/>
+      <c r="G78" s="68"/>
+      <c r="H78" s="68"/>
     </row>
     <row r="79" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="42"/>
@@ -2415,15 +2412,15 @@
       <c r="A80" s="21">
         <v>13</v>
       </c>
-      <c r="B80" s="56" t="s">
+      <c r="B80" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="C80" s="56"/>
-      <c r="D80" s="56"/>
-      <c r="E80" s="56"/>
-      <c r="F80" s="56"/>
-      <c r="G80" s="56"/>
-      <c r="H80" s="56"/>
+      <c r="C80" s="73"/>
+      <c r="D80" s="73"/>
+      <c r="E80" s="73"/>
+      <c r="F80" s="73"/>
+      <c r="G80" s="73"/>
+      <c r="H80" s="73"/>
     </row>
     <row r="81" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
@@ -2432,14 +2429,14 @@
       <c r="B81" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="C81" s="55" t="s">
+      <c r="C81" s="68" t="s">
         <v>111</v>
       </c>
-      <c r="D81" s="55"/>
-      <c r="E81" s="55"/>
-      <c r="F81" s="55"/>
-      <c r="G81" s="55"/>
-      <c r="H81" s="55"/>
+      <c r="D81" s="68"/>
+      <c r="E81" s="68"/>
+      <c r="F81" s="68"/>
+      <c r="G81" s="68"/>
+      <c r="H81" s="68"/>
     </row>
     <row r="82" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
@@ -2448,14 +2445,14 @@
       <c r="B82" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="C82" s="55" t="s">
+      <c r="C82" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="D82" s="55"/>
-      <c r="E82" s="55"/>
-      <c r="F82" s="55"/>
-      <c r="G82" s="55"/>
-      <c r="H82" s="55"/>
+      <c r="D82" s="68"/>
+      <c r="E82" s="68"/>
+      <c r="F82" s="68"/>
+      <c r="G82" s="68"/>
+      <c r="H82" s="68"/>
     </row>
     <row r="83" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="16" t="s">
@@ -2464,14 +2461,14 @@
       <c r="B83" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="C83" s="55" t="s">
+      <c r="C83" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="D83" s="55"/>
-      <c r="E83" s="55"/>
-      <c r="F83" s="55"/>
-      <c r="G83" s="55"/>
-      <c r="H83" s="55"/>
+      <c r="D83" s="68"/>
+      <c r="E83" s="68"/>
+      <c r="F83" s="68"/>
+      <c r="G83" s="68"/>
+      <c r="H83" s="68"/>
     </row>
     <row r="84" spans="1:8" s="6" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
@@ -2480,14 +2477,14 @@
       <c r="B84" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="C84" s="55" t="s">
+      <c r="C84" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="D84" s="55"/>
-      <c r="E84" s="55"/>
-      <c r="F84" s="55"/>
-      <c r="G84" s="55"/>
-      <c r="H84" s="55"/>
+      <c r="D84" s="68"/>
+      <c r="E84" s="68"/>
+      <c r="F84" s="68"/>
+      <c r="G84" s="68"/>
+      <c r="H84" s="68"/>
     </row>
     <row r="85" spans="1:8" s="6" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
@@ -2496,14 +2493,14 @@
       <c r="B85" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C85" s="55" t="s">
+      <c r="C85" s="68" t="s">
         <v>118</v>
       </c>
-      <c r="D85" s="55"/>
-      <c r="E85" s="55"/>
-      <c r="F85" s="55"/>
-      <c r="G85" s="55"/>
-      <c r="H85" s="55"/>
+      <c r="D85" s="68"/>
+      <c r="E85" s="68"/>
+      <c r="F85" s="68"/>
+      <c r="G85" s="68"/>
+      <c r="H85" s="68"/>
     </row>
     <row r="86" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="16" t="s">
@@ -2512,14 +2509,14 @@
       <c r="B86" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="C86" s="55" t="s">
+      <c r="C86" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="D86" s="55"/>
-      <c r="E86" s="55"/>
-      <c r="F86" s="55"/>
-      <c r="G86" s="55"/>
-      <c r="H86" s="55"/>
+      <c r="D86" s="68"/>
+      <c r="E86" s="68"/>
+      <c r="F86" s="68"/>
+      <c r="G86" s="68"/>
+      <c r="H86" s="68"/>
     </row>
     <row r="87" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="16" t="s">
@@ -2528,14 +2525,14 @@
       <c r="B87" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="C87" s="55" t="s">
+      <c r="C87" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="D87" s="55"/>
-      <c r="E87" s="55"/>
-      <c r="F87" s="55"/>
-      <c r="G87" s="55"/>
-      <c r="H87" s="55"/>
+      <c r="D87" s="68"/>
+      <c r="E87" s="68"/>
+      <c r="F87" s="68"/>
+      <c r="G87" s="68"/>
+      <c r="H87" s="68"/>
     </row>
     <row r="88" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="16" t="s">
@@ -2544,14 +2541,14 @@
       <c r="B88" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C88" s="55" t="s">
+      <c r="C88" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="D88" s="55"/>
-      <c r="E88" s="55"/>
-      <c r="F88" s="55"/>
-      <c r="G88" s="55"/>
-      <c r="H88" s="55"/>
+      <c r="D88" s="68"/>
+      <c r="E88" s="68"/>
+      <c r="F88" s="68"/>
+      <c r="G88" s="68"/>
+      <c r="H88" s="68"/>
     </row>
     <row r="89" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="16" t="s">
@@ -2560,14 +2557,14 @@
       <c r="B89" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="C89" s="55" t="s">
+      <c r="C89" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="D89" s="55"/>
-      <c r="E89" s="55"/>
-      <c r="F89" s="55"/>
-      <c r="G89" s="55"/>
-      <c r="H89" s="55"/>
+      <c r="D89" s="68"/>
+      <c r="E89" s="68"/>
+      <c r="F89" s="68"/>
+      <c r="G89" s="68"/>
+      <c r="H89" s="68"/>
     </row>
     <row r="90" spans="1:8" s="6" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="16" t="s">
@@ -2576,14 +2573,14 @@
       <c r="B90" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="C90" s="55" t="s">
+      <c r="C90" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="D90" s="55"/>
-      <c r="E90" s="55"/>
-      <c r="F90" s="55"/>
-      <c r="G90" s="55"/>
-      <c r="H90" s="55"/>
+      <c r="D90" s="68"/>
+      <c r="E90" s="68"/>
+      <c r="F90" s="68"/>
+      <c r="G90" s="68"/>
+      <c r="H90" s="68"/>
     </row>
     <row r="91" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="16" t="s">
@@ -2592,14 +2589,12 @@
       <c r="B91" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C91" s="55" t="s">
-        <v>132</v>
-      </c>
-      <c r="D91" s="55"/>
-      <c r="E91" s="55"/>
-      <c r="F91" s="55"/>
-      <c r="G91" s="55"/>
-      <c r="H91" s="55"/>
+      <c r="C91" s="68"/>
+      <c r="D91" s="68"/>
+      <c r="E91" s="68"/>
+      <c r="F91" s="68"/>
+      <c r="G91" s="68"/>
+      <c r="H91" s="68"/>
     </row>
     <row r="92" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="15"/>
@@ -2615,27 +2610,27 @@
       <c r="A93" s="21">
         <v>14</v>
       </c>
-      <c r="B93" s="54" t="s">
+      <c r="B93" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="C93" s="54"/>
-      <c r="D93" s="54"/>
-      <c r="E93" s="54"/>
-      <c r="F93" s="54"/>
-      <c r="G93" s="54"/>
-      <c r="H93" s="54"/>
+      <c r="C93" s="77"/>
+      <c r="D93" s="77"/>
+      <c r="E93" s="77"/>
+      <c r="F93" s="77"/>
+      <c r="G93" s="77"/>
+      <c r="H93" s="77"/>
     </row>
     <row r="94" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
-      <c r="B94" s="46" t="s">
+      <c r="B94" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="C94" s="47"/>
-      <c r="D94" s="47"/>
-      <c r="E94" s="47"/>
-      <c r="F94" s="47"/>
-      <c r="G94" s="47"/>
-      <c r="H94" s="48"/>
+      <c r="C94" s="70"/>
+      <c r="D94" s="70"/>
+      <c r="E94" s="70"/>
+      <c r="F94" s="70"/>
+      <c r="G94" s="70"/>
+      <c r="H94" s="71"/>
     </row>
     <row r="95" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="15"/>
@@ -2651,27 +2646,27 @@
       <c r="A96" s="45">
         <v>15</v>
       </c>
-      <c r="B96" s="49" t="s">
+      <c r="B96" s="78" t="s">
         <v>128</v>
       </c>
-      <c r="C96" s="49"/>
-      <c r="D96" s="49"/>
-      <c r="E96" s="49"/>
-      <c r="F96" s="49"/>
-      <c r="G96" s="49"/>
-      <c r="H96" s="49"/>
+      <c r="C96" s="78"/>
+      <c r="D96" s="78"/>
+      <c r="E96" s="78"/>
+      <c r="F96" s="78"/>
+      <c r="G96" s="78"/>
+      <c r="H96" s="78"/>
     </row>
     <row r="97" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
-      <c r="B97" s="46" t="s">
+      <c r="B97" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="C97" s="47"/>
-      <c r="D97" s="47"/>
-      <c r="E97" s="47"/>
-      <c r="F97" s="47"/>
-      <c r="G97" s="47"/>
-      <c r="H97" s="48"/>
+      <c r="C97" s="70"/>
+      <c r="D97" s="70"/>
+      <c r="E97" s="70"/>
+      <c r="F97" s="70"/>
+      <c r="G97" s="70"/>
+      <c r="H97" s="71"/>
     </row>
     <row r="98" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="15"/>
@@ -2687,27 +2682,27 @@
       <c r="A99" s="21">
         <v>16</v>
       </c>
-      <c r="B99" s="50" t="s">
+      <c r="B99" s="79" t="s">
         <v>130</v>
       </c>
-      <c r="C99" s="50"/>
-      <c r="D99" s="50"/>
-      <c r="E99" s="50"/>
-      <c r="F99" s="50"/>
-      <c r="G99" s="50"/>
-      <c r="H99" s="50"/>
+      <c r="C99" s="79"/>
+      <c r="D99" s="79"/>
+      <c r="E99" s="79"/>
+      <c r="F99" s="79"/>
+      <c r="G99" s="79"/>
+      <c r="H99" s="79"/>
     </row>
     <row r="100" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
-      <c r="B100" s="51" t="s">
+      <c r="B100" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="C100" s="52"/>
-      <c r="D100" s="52"/>
-      <c r="E100" s="52"/>
-      <c r="F100" s="52"/>
-      <c r="G100" s="52"/>
-      <c r="H100" s="53"/>
+      <c r="C100" s="81"/>
+      <c r="D100" s="81"/>
+      <c r="E100" s="81"/>
+      <c r="F100" s="81"/>
+      <c r="G100" s="81"/>
+      <c r="H100" s="82"/>
     </row>
     <row r="101" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="15"/>
@@ -2721,6 +2716,59 @@
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="B94:H94"/>
+    <mergeCell ref="B96:H96"/>
+    <mergeCell ref="B97:H97"/>
+    <mergeCell ref="B99:H99"/>
+    <mergeCell ref="B100:H100"/>
+    <mergeCell ref="B93:H93"/>
+    <mergeCell ref="C81:H81"/>
+    <mergeCell ref="C82:H82"/>
+    <mergeCell ref="C83:H83"/>
+    <mergeCell ref="C84:H84"/>
+    <mergeCell ref="C85:H85"/>
+    <mergeCell ref="C86:H86"/>
+    <mergeCell ref="C87:H87"/>
+    <mergeCell ref="C88:H88"/>
+    <mergeCell ref="C89:H89"/>
+    <mergeCell ref="C90:H90"/>
+    <mergeCell ref="C91:H91"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="C68:H68"/>
+    <mergeCell ref="C69:H69"/>
+    <mergeCell ref="C71:H71"/>
+    <mergeCell ref="C72:H72"/>
+    <mergeCell ref="C73:H73"/>
+    <mergeCell ref="C74:H74"/>
+    <mergeCell ref="C75:H75"/>
+    <mergeCell ref="C76:H76"/>
+    <mergeCell ref="C77:H77"/>
+    <mergeCell ref="C78:H78"/>
+    <mergeCell ref="C70:H70"/>
+    <mergeCell ref="C67:H67"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="D56:H56"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B62:H62"/>
+    <mergeCell ref="B64:H64"/>
+    <mergeCell ref="C65:H65"/>
+    <mergeCell ref="C66:H66"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="B39:H39"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="A3:H3"/>
@@ -2734,59 +2782,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="C67:H67"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="D56:H56"/>
-    <mergeCell ref="B58:H58"/>
-    <mergeCell ref="B59:H59"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="B62:H62"/>
-    <mergeCell ref="B64:H64"/>
-    <mergeCell ref="C65:H65"/>
-    <mergeCell ref="C66:H66"/>
-    <mergeCell ref="B80:H80"/>
-    <mergeCell ref="C68:H68"/>
-    <mergeCell ref="C69:H69"/>
-    <mergeCell ref="C71:H71"/>
-    <mergeCell ref="C72:H72"/>
-    <mergeCell ref="C73:H73"/>
-    <mergeCell ref="C74:H74"/>
-    <mergeCell ref="C75:H75"/>
-    <mergeCell ref="C76:H76"/>
-    <mergeCell ref="C77:H77"/>
-    <mergeCell ref="C78:H78"/>
-    <mergeCell ref="C70:H70"/>
-    <mergeCell ref="B93:H93"/>
-    <mergeCell ref="C81:H81"/>
-    <mergeCell ref="C82:H82"/>
-    <mergeCell ref="C83:H83"/>
-    <mergeCell ref="C84:H84"/>
-    <mergeCell ref="C85:H85"/>
-    <mergeCell ref="C86:H86"/>
-    <mergeCell ref="C87:H87"/>
-    <mergeCell ref="C88:H88"/>
-    <mergeCell ref="C89:H89"/>
-    <mergeCell ref="C90:H90"/>
-    <mergeCell ref="C91:H91"/>
-    <mergeCell ref="B94:H94"/>
-    <mergeCell ref="B96:H96"/>
-    <mergeCell ref="B97:H97"/>
-    <mergeCell ref="B99:H99"/>
-    <mergeCell ref="B100:H100"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Added code to make it loop faster and decreased the size of the code
</commit_message>
<xml_diff>
--- a/SummerWork/All_Reports/Adrian_SD_61_2017-2018_Outdoor_School_Report.xlsx
+++ b/SummerWork/All_Reports/Adrian_SD_61_2017-2018_Outdoor_School_Report.xlsx
@@ -804,6 +804,96 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -813,9 +903,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -827,93 +914,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1208,8 +1208,8 @@
   </sheetPr>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="63" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81:H81"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="63" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91:H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1226,15 +1226,15 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -1251,28 +1251,28 @@
       <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
@@ -1288,15 +1288,15 @@
       <c r="A6" s="14">
         <v>1</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
@@ -1312,69 +1312,69 @@
       <c r="A8" s="16">
         <v>2</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="51"/>
+      <c r="D9" s="80"/>
       <c r="E9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="52"/>
-      <c r="H9" s="51"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="80"/>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="51"/>
+      <c r="D10" s="80"/>
       <c r="E10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="52"/>
-      <c r="H10" s="51"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="80"/>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="51"/>
+      <c r="D11" s="80"/>
       <c r="E11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="52"/>
-      <c r="H11" s="51"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="80"/>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
@@ -1404,66 +1404,66 @@
       <c r="A14" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
     </row>
     <row r="17" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
     </row>
     <row r="18" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="57"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="68"/>
       <c r="G18" s="22">
         <v>5</v>
       </c>
@@ -1474,13 +1474,13 @@
     </row>
     <row r="19" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="59"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="70"/>
       <c r="G19" s="22">
         <v>3</v>
       </c>
@@ -1491,13 +1491,13 @@
     </row>
     <row r="20" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="59"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="70"/>
       <c r="G20" s="22">
         <v>4</v>
       </c>
@@ -1508,13 +1508,13 @@
     </row>
     <row r="21" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="59"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="70"/>
       <c r="G21" s="22">
         <v>5</v>
       </c>
@@ -1525,13 +1525,13 @@
     </row>
     <row r="22" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="59"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="70"/>
       <c r="G22" s="22">
         <v>5</v>
       </c>
@@ -1572,15 +1572,15 @@
     </row>
     <row r="25" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
@@ -1758,30 +1758,30 @@
       <c r="A35" s="21">
         <v>5</v>
       </c>
-      <c r="B35" s="61" t="s">
+      <c r="B35" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
       <c r="I35" s="23"/>
       <c r="J35" s="23"/>
       <c r="K35" s="23"/>
     </row>
     <row r="36" spans="1:11" s="6" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
-      <c r="B36" s="62" t="s">
+      <c r="B36" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="64"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="62"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
@@ -1818,15 +1818,15 @@
     </row>
     <row r="39" spans="1:11" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
-      <c r="B39" s="65" t="s">
+      <c r="B39" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="66"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="66"/>
-      <c r="G39" s="66"/>
-      <c r="H39" s="67"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="75"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
@@ -1848,30 +1848,30 @@
       <c r="A41" s="21">
         <v>7</v>
       </c>
-      <c r="B41" s="54" t="s">
+      <c r="B41" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="54"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="54"/>
-      <c r="H41" s="54"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
     </row>
     <row r="42" spans="1:11" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
-      <c r="B42" s="62" t="s">
+      <c r="B42" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="64"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="62"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
@@ -1893,30 +1893,30 @@
       <c r="A44" s="21">
         <v>8</v>
       </c>
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="54"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="54"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
     </row>
     <row r="45" spans="1:11" s="6" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
-      <c r="B45" s="62" t="s">
+      <c r="B45" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
-      <c r="G45" s="63"/>
-      <c r="H45" s="64"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="62"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
@@ -2070,13 +2070,13 @@
       <c r="A56" s="13"/>
       <c r="B56" s="12"/>
       <c r="C56" s="20"/>
-      <c r="D56" s="69" t="s">
+      <c r="D56" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="E56" s="70"/>
-      <c r="F56" s="70"/>
-      <c r="G56" s="70"/>
-      <c r="H56" s="71"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="48"/>
     </row>
     <row r="57" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
@@ -2092,27 +2092,27 @@
       <c r="A58" s="21">
         <v>10</v>
       </c>
-      <c r="B58" s="54" t="s">
+      <c r="B58" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="54"/>
-      <c r="D58" s="54"/>
-      <c r="E58" s="54"/>
-      <c r="F58" s="54"/>
-      <c r="G58" s="54"/>
-      <c r="H58" s="54"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63"/>
+      <c r="E58" s="63"/>
+      <c r="F58" s="63"/>
+      <c r="G58" s="63"/>
+      <c r="H58" s="63"/>
     </row>
     <row r="59" spans="1:8" s="6" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
-      <c r="B59" s="62" t="s">
+      <c r="B59" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="63"/>
-      <c r="D59" s="63"/>
-      <c r="E59" s="63"/>
-      <c r="F59" s="63"/>
-      <c r="G59" s="63"/>
-      <c r="H59" s="64"/>
+      <c r="C59" s="61"/>
+      <c r="D59" s="61"/>
+      <c r="E59" s="61"/>
+      <c r="F59" s="61"/>
+      <c r="G59" s="61"/>
+      <c r="H59" s="62"/>
     </row>
     <row r="60" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
@@ -2128,27 +2128,27 @@
       <c r="A61" s="21">
         <v>11</v>
       </c>
-      <c r="B61" s="54" t="s">
+      <c r="B61" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="54"/>
-      <c r="D61" s="54"/>
-      <c r="E61" s="54"/>
-      <c r="F61" s="54"/>
-      <c r="G61" s="54"/>
-      <c r="H61" s="54"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="63"/>
+      <c r="F61" s="63"/>
+      <c r="G61" s="63"/>
+      <c r="H61" s="63"/>
     </row>
     <row r="62" spans="1:8" s="6" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
-      <c r="B62" s="62" t="s">
+      <c r="B62" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="63"/>
-      <c r="D62" s="63"/>
-      <c r="E62" s="63"/>
-      <c r="F62" s="63"/>
-      <c r="G62" s="63"/>
-      <c r="H62" s="64"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="61"/>
+      <c r="F62" s="61"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="62"/>
     </row>
     <row r="63" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
@@ -2164,15 +2164,15 @@
       <c r="A64" s="36">
         <v>12</v>
       </c>
-      <c r="B64" s="54" t="s">
+      <c r="B64" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="54"/>
-      <c r="D64" s="54"/>
-      <c r="E64" s="54"/>
-      <c r="F64" s="54"/>
-      <c r="G64" s="54"/>
-      <c r="H64" s="54"/>
+      <c r="C64" s="63"/>
+      <c r="D64" s="63"/>
+      <c r="E64" s="63"/>
+      <c r="F64" s="63"/>
+      <c r="G64" s="63"/>
+      <c r="H64" s="63"/>
     </row>
     <row r="65" spans="1:8" s="6" customFormat="1" ht="86.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
@@ -2181,14 +2181,14 @@
       <c r="B65" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="72" t="s">
+      <c r="C65" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="72"/>
-      <c r="H65" s="72"/>
+      <c r="D65" s="64"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="64"/>
+      <c r="H65" s="64"/>
     </row>
     <row r="66" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
@@ -2197,14 +2197,14 @@
       <c r="B66" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="68" t="s">
+      <c r="C66" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="D66" s="68"/>
-      <c r="E66" s="68"/>
-      <c r="F66" s="68"/>
-      <c r="G66" s="68"/>
-      <c r="H66" s="68"/>
+      <c r="D66" s="55"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="55"/>
+      <c r="G66" s="55"/>
+      <c r="H66" s="55"/>
     </row>
     <row r="67" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
@@ -2213,14 +2213,14 @@
       <c r="B67" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C67" s="68" t="s">
+      <c r="C67" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="D67" s="68"/>
-      <c r="E67" s="68"/>
-      <c r="F67" s="68"/>
-      <c r="G67" s="68"/>
-      <c r="H67" s="68"/>
+      <c r="D67" s="55"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="55"/>
+      <c r="G67" s="55"/>
+      <c r="H67" s="55"/>
     </row>
     <row r="68" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
@@ -2229,14 +2229,14 @@
       <c r="B68" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="D68" s="68"/>
-      <c r="E68" s="68"/>
-      <c r="F68" s="68"/>
-      <c r="G68" s="68"/>
-      <c r="H68" s="68"/>
+      <c r="D68" s="55"/>
+      <c r="E68" s="55"/>
+      <c r="F68" s="55"/>
+      <c r="G68" s="55"/>
+      <c r="H68" s="55"/>
     </row>
     <row r="69" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
@@ -2245,14 +2245,14 @@
       <c r="B69" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="C69" s="68" t="s">
+      <c r="C69" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="D69" s="68"/>
-      <c r="E69" s="68"/>
-      <c r="F69" s="68"/>
-      <c r="G69" s="68"/>
-      <c r="H69" s="68"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="55"/>
+      <c r="G69" s="55"/>
+      <c r="H69" s="55"/>
     </row>
     <row r="70" spans="1:8" s="6" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
@@ -2261,14 +2261,14 @@
       <c r="B70" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="C70" s="74" t="s">
+      <c r="C70" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="D70" s="75"/>
-      <c r="E70" s="75"/>
-      <c r="F70" s="75"/>
-      <c r="G70" s="75"/>
-      <c r="H70" s="76"/>
+      <c r="D70" s="58"/>
+      <c r="E70" s="58"/>
+      <c r="F70" s="58"/>
+      <c r="G70" s="58"/>
+      <c r="H70" s="59"/>
     </row>
     <row r="71" spans="1:8" s="6" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
@@ -2277,14 +2277,14 @@
       <c r="B71" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="C71" s="68" t="s">
+      <c r="C71" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="D71" s="68"/>
-      <c r="E71" s="68"/>
-      <c r="F71" s="68"/>
-      <c r="G71" s="68"/>
-      <c r="H71" s="68"/>
+      <c r="D71" s="55"/>
+      <c r="E71" s="55"/>
+      <c r="F71" s="55"/>
+      <c r="G71" s="55"/>
+      <c r="H71" s="55"/>
     </row>
     <row r="72" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
@@ -2293,14 +2293,14 @@
       <c r="B72" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C72" s="68" t="s">
+      <c r="C72" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="D72" s="68"/>
-      <c r="E72" s="68"/>
-      <c r="F72" s="68"/>
-      <c r="G72" s="68"/>
-      <c r="H72" s="68"/>
+      <c r="D72" s="55"/>
+      <c r="E72" s="55"/>
+      <c r="F72" s="55"/>
+      <c r="G72" s="55"/>
+      <c r="H72" s="55"/>
     </row>
     <row r="73" spans="1:8" s="6" customFormat="1" ht="66.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
@@ -2309,14 +2309,14 @@
       <c r="B73" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="D73" s="68"/>
-      <c r="E73" s="68"/>
-      <c r="F73" s="68"/>
-      <c r="G73" s="68"/>
-      <c r="H73" s="68"/>
+      <c r="D73" s="55"/>
+      <c r="E73" s="55"/>
+      <c r="F73" s="55"/>
+      <c r="G73" s="55"/>
+      <c r="H73" s="55"/>
     </row>
     <row r="74" spans="1:8" s="6" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
@@ -2325,14 +2325,14 @@
       <c r="B74" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="C74" s="68" t="s">
+      <c r="C74" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="D74" s="68"/>
-      <c r="E74" s="68"/>
-      <c r="F74" s="68"/>
-      <c r="G74" s="68"/>
-      <c r="H74" s="68"/>
+      <c r="D74" s="55"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="55"/>
+      <c r="G74" s="55"/>
+      <c r="H74" s="55"/>
     </row>
     <row r="75" spans="1:8" s="6" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
@@ -2341,14 +2341,14 @@
       <c r="B75" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="C75" s="68" t="s">
+      <c r="C75" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="D75" s="68"/>
-      <c r="E75" s="68"/>
-      <c r="F75" s="68"/>
-      <c r="G75" s="68"/>
-      <c r="H75" s="68"/>
+      <c r="D75" s="55"/>
+      <c r="E75" s="55"/>
+      <c r="F75" s="55"/>
+      <c r="G75" s="55"/>
+      <c r="H75" s="55"/>
     </row>
     <row r="76" spans="1:8" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
@@ -2357,14 +2357,14 @@
       <c r="B76" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="C76" s="68" t="s">
+      <c r="C76" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="D76" s="68"/>
-      <c r="E76" s="68"/>
-      <c r="F76" s="68"/>
-      <c r="G76" s="68"/>
-      <c r="H76" s="68"/>
+      <c r="D76" s="55"/>
+      <c r="E76" s="55"/>
+      <c r="F76" s="55"/>
+      <c r="G76" s="55"/>
+      <c r="H76" s="55"/>
     </row>
     <row r="77" spans="1:8" s="6" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
@@ -2373,14 +2373,14 @@
       <c r="B77" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="C77" s="68" t="s">
+      <c r="C77" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="D77" s="68"/>
-      <c r="E77" s="68"/>
-      <c r="F77" s="68"/>
-      <c r="G77" s="68"/>
-      <c r="H77" s="68"/>
+      <c r="D77" s="55"/>
+      <c r="E77" s="55"/>
+      <c r="F77" s="55"/>
+      <c r="G77" s="55"/>
+      <c r="H77" s="55"/>
     </row>
     <row r="78" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
@@ -2389,14 +2389,14 @@
       <c r="B78" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="D78" s="68"/>
-      <c r="E78" s="68"/>
-      <c r="F78" s="68"/>
-      <c r="G78" s="68"/>
-      <c r="H78" s="68"/>
+      <c r="D78" s="55"/>
+      <c r="E78" s="55"/>
+      <c r="F78" s="55"/>
+      <c r="G78" s="55"/>
+      <c r="H78" s="55"/>
     </row>
     <row r="79" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="42"/>
@@ -2412,15 +2412,15 @@
       <c r="A80" s="21">
         <v>13</v>
       </c>
-      <c r="B80" s="73" t="s">
+      <c r="B80" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="C80" s="73"/>
-      <c r="D80" s="73"/>
-      <c r="E80" s="73"/>
-      <c r="F80" s="73"/>
-      <c r="G80" s="73"/>
-      <c r="H80" s="73"/>
+      <c r="C80" s="56"/>
+      <c r="D80" s="56"/>
+      <c r="E80" s="56"/>
+      <c r="F80" s="56"/>
+      <c r="G80" s="56"/>
+      <c r="H80" s="56"/>
     </row>
     <row r="81" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
@@ -2429,14 +2429,14 @@
       <c r="B81" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="C81" s="68" t="s">
+      <c r="C81" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="D81" s="68"/>
-      <c r="E81" s="68"/>
-      <c r="F81" s="68"/>
-      <c r="G81" s="68"/>
-      <c r="H81" s="68"/>
+      <c r="D81" s="55"/>
+      <c r="E81" s="55"/>
+      <c r="F81" s="55"/>
+      <c r="G81" s="55"/>
+      <c r="H81" s="55"/>
     </row>
     <row r="82" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
@@ -2445,14 +2445,14 @@
       <c r="B82" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="C82" s="68" t="s">
+      <c r="C82" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="D82" s="68"/>
-      <c r="E82" s="68"/>
-      <c r="F82" s="68"/>
-      <c r="G82" s="68"/>
-      <c r="H82" s="68"/>
+      <c r="D82" s="55"/>
+      <c r="E82" s="55"/>
+      <c r="F82" s="55"/>
+      <c r="G82" s="55"/>
+      <c r="H82" s="55"/>
     </row>
     <row r="83" spans="1:8" s="6" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="16" t="s">
@@ -2461,14 +2461,14 @@
       <c r="B83" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="C83" s="68" t="s">
+      <c r="C83" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="D83" s="68"/>
-      <c r="E83" s="68"/>
-      <c r="F83" s="68"/>
-      <c r="G83" s="68"/>
-      <c r="H83" s="68"/>
+      <c r="D83" s="55"/>
+      <c r="E83" s="55"/>
+      <c r="F83" s="55"/>
+      <c r="G83" s="55"/>
+      <c r="H83" s="55"/>
     </row>
     <row r="84" spans="1:8" s="6" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
@@ -2477,14 +2477,14 @@
       <c r="B84" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="C84" s="68" t="s">
+      <c r="C84" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="D84" s="68"/>
-      <c r="E84" s="68"/>
-      <c r="F84" s="68"/>
-      <c r="G84" s="68"/>
-      <c r="H84" s="68"/>
+      <c r="D84" s="55"/>
+      <c r="E84" s="55"/>
+      <c r="F84" s="55"/>
+      <c r="G84" s="55"/>
+      <c r="H84" s="55"/>
     </row>
     <row r="85" spans="1:8" s="6" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
@@ -2493,14 +2493,14 @@
       <c r="B85" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C85" s="68" t="s">
+      <c r="C85" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="D85" s="68"/>
-      <c r="E85" s="68"/>
-      <c r="F85" s="68"/>
-      <c r="G85" s="68"/>
-      <c r="H85" s="68"/>
+      <c r="D85" s="55"/>
+      <c r="E85" s="55"/>
+      <c r="F85" s="55"/>
+      <c r="G85" s="55"/>
+      <c r="H85" s="55"/>
     </row>
     <row r="86" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="16" t="s">
@@ -2509,14 +2509,14 @@
       <c r="B86" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="C86" s="68" t="s">
+      <c r="C86" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="D86" s="68"/>
-      <c r="E86" s="68"/>
-      <c r="F86" s="68"/>
-      <c r="G86" s="68"/>
-      <c r="H86" s="68"/>
+      <c r="D86" s="55"/>
+      <c r="E86" s="55"/>
+      <c r="F86" s="55"/>
+      <c r="G86" s="55"/>
+      <c r="H86" s="55"/>
     </row>
     <row r="87" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="16" t="s">
@@ -2525,14 +2525,14 @@
       <c r="B87" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="C87" s="68" t="s">
+      <c r="C87" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="D87" s="68"/>
-      <c r="E87" s="68"/>
-      <c r="F87" s="68"/>
-      <c r="G87" s="68"/>
-      <c r="H87" s="68"/>
+      <c r="D87" s="55"/>
+      <c r="E87" s="55"/>
+      <c r="F87" s="55"/>
+      <c r="G87" s="55"/>
+      <c r="H87" s="55"/>
     </row>
     <row r="88" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="16" t="s">
@@ -2541,14 +2541,14 @@
       <c r="B88" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C88" s="68" t="s">
+      <c r="C88" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="D88" s="68"/>
-      <c r="E88" s="68"/>
-      <c r="F88" s="68"/>
-      <c r="G88" s="68"/>
-      <c r="H88" s="68"/>
+      <c r="D88" s="55"/>
+      <c r="E88" s="55"/>
+      <c r="F88" s="55"/>
+      <c r="G88" s="55"/>
+      <c r="H88" s="55"/>
     </row>
     <row r="89" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="16" t="s">
@@ -2557,14 +2557,14 @@
       <c r="B89" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="C89" s="68" t="s">
+      <c r="C89" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="D89" s="68"/>
-      <c r="E89" s="68"/>
-      <c r="F89" s="68"/>
-      <c r="G89" s="68"/>
-      <c r="H89" s="68"/>
+      <c r="D89" s="55"/>
+      <c r="E89" s="55"/>
+      <c r="F89" s="55"/>
+      <c r="G89" s="55"/>
+      <c r="H89" s="55"/>
     </row>
     <row r="90" spans="1:8" s="6" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="16" t="s">
@@ -2573,14 +2573,14 @@
       <c r="B90" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="C90" s="68" t="s">
+      <c r="C90" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="D90" s="68"/>
-      <c r="E90" s="68"/>
-      <c r="F90" s="68"/>
-      <c r="G90" s="68"/>
-      <c r="H90" s="68"/>
+      <c r="D90" s="55"/>
+      <c r="E90" s="55"/>
+      <c r="F90" s="55"/>
+      <c r="G90" s="55"/>
+      <c r="H90" s="55"/>
     </row>
     <row r="91" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="16" t="s">
@@ -2589,12 +2589,12 @@
       <c r="B91" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C91" s="68"/>
-      <c r="D91" s="68"/>
-      <c r="E91" s="68"/>
-      <c r="F91" s="68"/>
-      <c r="G91" s="68"/>
-      <c r="H91" s="68"/>
+      <c r="C91" s="55"/>
+      <c r="D91" s="55"/>
+      <c r="E91" s="55"/>
+      <c r="F91" s="55"/>
+      <c r="G91" s="55"/>
+      <c r="H91" s="55"/>
     </row>
     <row r="92" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="15"/>
@@ -2610,27 +2610,27 @@
       <c r="A93" s="21">
         <v>14</v>
       </c>
-      <c r="B93" s="77" t="s">
+      <c r="B93" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="C93" s="77"/>
-      <c r="D93" s="77"/>
-      <c r="E93" s="77"/>
-      <c r="F93" s="77"/>
-      <c r="G93" s="77"/>
-      <c r="H93" s="77"/>
+      <c r="C93" s="54"/>
+      <c r="D93" s="54"/>
+      <c r="E93" s="54"/>
+      <c r="F93" s="54"/>
+      <c r="G93" s="54"/>
+      <c r="H93" s="54"/>
     </row>
     <row r="94" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
-      <c r="B94" s="69" t="s">
+      <c r="B94" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C94" s="70"/>
-      <c r="D94" s="70"/>
-      <c r="E94" s="70"/>
-      <c r="F94" s="70"/>
-      <c r="G94" s="70"/>
-      <c r="H94" s="71"/>
+      <c r="C94" s="47"/>
+      <c r="D94" s="47"/>
+      <c r="E94" s="47"/>
+      <c r="F94" s="47"/>
+      <c r="G94" s="47"/>
+      <c r="H94" s="48"/>
     </row>
     <row r="95" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="15"/>
@@ -2646,27 +2646,27 @@
       <c r="A96" s="45">
         <v>15</v>
       </c>
-      <c r="B96" s="78" t="s">
+      <c r="B96" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="C96" s="78"/>
-      <c r="D96" s="78"/>
-      <c r="E96" s="78"/>
-      <c r="F96" s="78"/>
-      <c r="G96" s="78"/>
-      <c r="H96" s="78"/>
+      <c r="C96" s="49"/>
+      <c r="D96" s="49"/>
+      <c r="E96" s="49"/>
+      <c r="F96" s="49"/>
+      <c r="G96" s="49"/>
+      <c r="H96" s="49"/>
     </row>
     <row r="97" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
-      <c r="B97" s="69" t="s">
+      <c r="B97" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C97" s="70"/>
-      <c r="D97" s="70"/>
-      <c r="E97" s="70"/>
-      <c r="F97" s="70"/>
-      <c r="G97" s="70"/>
-      <c r="H97" s="71"/>
+      <c r="C97" s="47"/>
+      <c r="D97" s="47"/>
+      <c r="E97" s="47"/>
+      <c r="F97" s="47"/>
+      <c r="G97" s="47"/>
+      <c r="H97" s="48"/>
     </row>
     <row r="98" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="15"/>
@@ -2682,27 +2682,27 @@
       <c r="A99" s="21">
         <v>16</v>
       </c>
-      <c r="B99" s="79" t="s">
+      <c r="B99" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="C99" s="79"/>
-      <c r="D99" s="79"/>
-      <c r="E99" s="79"/>
-      <c r="F99" s="79"/>
-      <c r="G99" s="79"/>
-      <c r="H99" s="79"/>
+      <c r="C99" s="50"/>
+      <c r="D99" s="50"/>
+      <c r="E99" s="50"/>
+      <c r="F99" s="50"/>
+      <c r="G99" s="50"/>
+      <c r="H99" s="50"/>
     </row>
     <row r="100" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
-      <c r="B100" s="80" t="s">
+      <c r="B100" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="C100" s="81"/>
-      <c r="D100" s="81"/>
-      <c r="E100" s="81"/>
-      <c r="F100" s="81"/>
-      <c r="G100" s="81"/>
-      <c r="H100" s="82"/>
+      <c r="C100" s="52"/>
+      <c r="D100" s="52"/>
+      <c r="E100" s="52"/>
+      <c r="F100" s="52"/>
+      <c r="G100" s="52"/>
+      <c r="H100" s="53"/>
     </row>
     <row r="101" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="15"/>
@@ -2716,59 +2716,6 @@
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="B94:H94"/>
-    <mergeCell ref="B96:H96"/>
-    <mergeCell ref="B97:H97"/>
-    <mergeCell ref="B99:H99"/>
-    <mergeCell ref="B100:H100"/>
-    <mergeCell ref="B93:H93"/>
-    <mergeCell ref="C81:H81"/>
-    <mergeCell ref="C82:H82"/>
-    <mergeCell ref="C83:H83"/>
-    <mergeCell ref="C84:H84"/>
-    <mergeCell ref="C85:H85"/>
-    <mergeCell ref="C86:H86"/>
-    <mergeCell ref="C87:H87"/>
-    <mergeCell ref="C88:H88"/>
-    <mergeCell ref="C89:H89"/>
-    <mergeCell ref="C90:H90"/>
-    <mergeCell ref="C91:H91"/>
-    <mergeCell ref="B80:H80"/>
-    <mergeCell ref="C68:H68"/>
-    <mergeCell ref="C69:H69"/>
-    <mergeCell ref="C71:H71"/>
-    <mergeCell ref="C72:H72"/>
-    <mergeCell ref="C73:H73"/>
-    <mergeCell ref="C74:H74"/>
-    <mergeCell ref="C75:H75"/>
-    <mergeCell ref="C76:H76"/>
-    <mergeCell ref="C77:H77"/>
-    <mergeCell ref="C78:H78"/>
-    <mergeCell ref="C70:H70"/>
-    <mergeCell ref="C67:H67"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="D56:H56"/>
-    <mergeCell ref="B58:H58"/>
-    <mergeCell ref="B59:H59"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="B62:H62"/>
-    <mergeCell ref="B64:H64"/>
-    <mergeCell ref="C65:H65"/>
-    <mergeCell ref="C66:H66"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="B39:H39"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="A3:H3"/>
@@ -2782,6 +2729,59 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="C67:H67"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="D56:H56"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B62:H62"/>
+    <mergeCell ref="B64:H64"/>
+    <mergeCell ref="C65:H65"/>
+    <mergeCell ref="C66:H66"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="C68:H68"/>
+    <mergeCell ref="C69:H69"/>
+    <mergeCell ref="C71:H71"/>
+    <mergeCell ref="C72:H72"/>
+    <mergeCell ref="C73:H73"/>
+    <mergeCell ref="C74:H74"/>
+    <mergeCell ref="C75:H75"/>
+    <mergeCell ref="C76:H76"/>
+    <mergeCell ref="C77:H77"/>
+    <mergeCell ref="C78:H78"/>
+    <mergeCell ref="C70:H70"/>
+    <mergeCell ref="B93:H93"/>
+    <mergeCell ref="C81:H81"/>
+    <mergeCell ref="C82:H82"/>
+    <mergeCell ref="C83:H83"/>
+    <mergeCell ref="C84:H84"/>
+    <mergeCell ref="C85:H85"/>
+    <mergeCell ref="C86:H86"/>
+    <mergeCell ref="C87:H87"/>
+    <mergeCell ref="C88:H88"/>
+    <mergeCell ref="C89:H89"/>
+    <mergeCell ref="C90:H90"/>
+    <mergeCell ref="C91:H91"/>
+    <mergeCell ref="B94:H94"/>
+    <mergeCell ref="B96:H96"/>
+    <mergeCell ref="B97:H97"/>
+    <mergeCell ref="B99:H99"/>
+    <mergeCell ref="B100:H100"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="2">

</xml_diff>